<commit_message>
New liquidity spreadsheet V5
</commit_message>
<xml_diff>
--- a/_static/LP_rewards.xlsx
+++ b/_static/LP_rewards.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Equations" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t xml:space="preserve">* Only Update cells highlighted in yellow</t>
   </si>
@@ -135,54 +134,22 @@
   </si>
   <si>
     <t xml:space="preserve">VOL/TOTAL LOCKED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impermanent_loss = 2 * sqrt(price_ratio) / (1+price_ratio) — 1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DON'T USE THIS SHEET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L = 2 * SQRT(R)/(1+R) - 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANY should stay between</t>
-  </si>
-  <si>
-    <t xml:space="preserve">and</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSN should stay between</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USDT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="0%"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="0"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="0"/>
+    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -266,7 +233,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,10 +254,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,11 +262,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,15 +274,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,18 +295,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,13 +317,13 @@
   </sheetPr>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
@@ -390,7 +345,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>4810678.107058</v>
+        <v>4895043.469844</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>2</v>
@@ -401,7 +356,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>2064251.953969</v>
+        <v>2122096.595027</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>3</v>
@@ -413,7 +368,7 @@
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B4/B5</f>
-        <v>2.33047041462568</v>
+        <v>2.30670153343407</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>2</v>
@@ -433,7 +388,7 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">16500*B7*B4/(2*B4+B22+B40)</f>
-        <v>14982.0354148053</v>
+        <v>15005.3035618899</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>3</v>
@@ -444,7 +399,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>5.23</v>
+        <v>5.91</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>8</v>
@@ -457,9 +412,9 @@
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="0" t="n">
         <f aca="false">0.003*B9*1000000</f>
-        <v>15690</v>
+        <v>17730</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>2</v>
@@ -474,7 +429,7 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+B6*B8</f>
-        <v>50605.1902850779</v>
+        <v>52342.7567358552</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>2</v>
@@ -484,18 +439,18 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
-        <f aca="false">B11/B4/2</f>
-        <v>0.00525967328918062</v>
+      <c r="B12" s="5" t="n">
+        <f aca="false">B11/(B4*2)</f>
+        <v>0.00534650581331031</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="6" t="n">
         <f aca="false">B12*365</f>
-        <v>1.91978075055093</v>
+        <v>1.95147462185826</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>15</v>
@@ -505,7 +460,7 @@
       <c r="A14" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="7" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -513,9 +468,9 @@
       <c r="A15" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="8" t="n">
         <f aca="false">B6*B8*B14</f>
-        <v>34.9151902850779</v>
+        <v>34.6127567358552</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>2</v>
@@ -525,9 +480,9 @@
       <c r="A16" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="8" t="n">
         <f aca="false">B10*B14</f>
-        <v>15.69</v>
+        <v>17.73</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>2</v>
@@ -537,22 +492,22 @@
       <c r="A17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="8" t="n">
         <f aca="false">B11*B14</f>
-        <v>50.6051902850779</v>
+        <v>52.3427567358552</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
@@ -564,20 +519,20 @@
         <v>2</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>550597.753797</v>
+        <v>521070.886676</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>245080.272407</v>
-      </c>
-      <c r="C23" s="10" t="s">
+        <v>237713.211398</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -587,9 +542,9 @@
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B23/B22</f>
-        <v>0.44511673125597</v>
-      </c>
-      <c r="C24" s="10" t="s">
+        <v>0.456201291372107</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -600,7 +555,7 @@
       <c r="B25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -608,7 +563,7 @@
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">16500*B25*B22/(B22+2*B4+B40)</f>
-        <v>857.371337587132</v>
+        <v>798.647333777988</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>3</v>
@@ -619,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>2.34</v>
+        <v>1.39</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>8</v>
@@ -632,9 +587,9 @@
       <c r="A28" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="0" t="n">
         <f aca="false">0.003*B27*1000000</f>
-        <v>7020</v>
+        <v>4170</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>2</v>
@@ -649,7 +604,7 @@
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">B28+B6*B26</f>
-        <v>9018.07853659486</v>
+        <v>6012.24102949872</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>2</v>
@@ -659,18 +614,18 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="6" t="n">
-        <f aca="false">B29/B22*B6/2</f>
-        <v>0.0190850444642875</v>
+      <c r="B30" s="5" t="n">
+        <f aca="false">B29/(B22*2)</f>
+        <v>0.0057691200787016</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="7" t="n">
+      <c r="B31" s="6" t="n">
         <f aca="false">B30*365</f>
-        <v>6.96604122946494</v>
+        <v>2.10572882872608</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>15</v>
@@ -680,7 +635,7 @@
       <c r="A32" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="7" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -688,9 +643,9 @@
       <c r="A33" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="9" t="n">
+      <c r="B33" s="8" t="n">
         <f aca="false">B6*B26*B32</f>
-        <v>1.99807853659486</v>
+        <v>1.84224102949872</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>2</v>
@@ -700,9 +655,9 @@
       <c r="A34" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="9" t="n">
+      <c r="B34" s="8" t="n">
         <f aca="false">B28*B32</f>
-        <v>7.02</v>
+        <v>4.17</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>2</v>
@@ -712,16 +667,16 @@
       <c r="A35" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="9" t="n">
+      <c r="B35" s="8" t="n">
         <f aca="false">B29*B32</f>
-        <v>9.01807853659486</v>
+        <v>6.01224102949872</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="9"/>
+      <c r="B36" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
@@ -733,53 +688,53 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>424228.26885</v>
+        <v>454131.515407</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>532.259424</v>
-      </c>
-      <c r="C41" s="10" t="s">
+        <v>567.912245</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="5" t="n">
+      <c r="B42" s="0" t="n">
         <f aca="false">B40/B41</f>
-        <v>797.03289358762</v>
-      </c>
-      <c r="C42" s="10"/>
+        <v>799.650860507507</v>
+      </c>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="5" t="n">
+      <c r="B43" s="0" t="n">
         <f aca="false">B42*B24</f>
-        <v>354.772676297209</v>
-      </c>
-      <c r="C43" s="10" t="s">
+        <v>364.801755210341</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="10"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -787,7 +742,7 @@
       </c>
       <c r="B45" s="0" t="n">
         <f aca="false">16500*B44*B40/(B40+2*B4+B22)</f>
-        <v>660.593247607578</v>
+        <v>696.04910433209</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>3</v>
@@ -798,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>2.32</v>
+        <v>1.88</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>8</v>
@@ -811,9 +766,9 @@
       <c r="A47" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="5" t="n">
+      <c r="B47" s="0" t="n">
         <f aca="false">0.003*B46*1000000</f>
-        <v>6960</v>
+        <v>5640</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>2</v>
@@ -828,7 +783,7 @@
       </c>
       <c r="B48" s="0" t="n">
         <f aca="false">B47+B6*B45</f>
-        <v>8499.49301965096</v>
+        <v>7245.57753630824</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>2</v>
@@ -838,18 +793,18 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="6" t="n">
-        <f aca="false">B48/B40*B27/2</f>
-        <v>0.0234411696795901</v>
+      <c r="B49" s="5" t="n">
+        <f aca="false">B48/(B40*2)</f>
+        <v>0.00797740003775629</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="7" t="n">
+      <c r="B50" s="6" t="n">
         <f aca="false">B49*365</f>
-        <v>8.55602693305039</v>
+        <v>2.91175101378104</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>15</v>
@@ -859,7 +814,7 @@
       <c r="A51" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="8" t="n">
+      <c r="B51" s="7" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -867,9 +822,9 @@
       <c r="A52" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="9" t="n">
+      <c r="B52" s="8" t="n">
         <f aca="false">B6*B45*B51</f>
-        <v>1.53949301965096</v>
+        <v>1.60557753630824</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>2</v>
@@ -879,9 +834,9 @@
       <c r="A53" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="9" t="n">
+      <c r="B53" s="8" t="n">
         <f aca="false">B47*B51</f>
-        <v>6.96</v>
+        <v>5.64</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>2</v>
@@ -891,9 +846,9 @@
       <c r="A54" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="9" t="n">
+      <c r="B54" s="8" t="n">
         <f aca="false">B48*B51</f>
-        <v>8.49949301965096</v>
+        <v>7.24557753630824</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>2</v>
@@ -904,9 +859,9 @@
       <c r="A58" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="11" t="n">
+      <c r="B58" s="10" t="n">
         <f aca="false">B15+B33+B52</f>
-        <v>38.4527618413237</v>
+        <v>38.0605753016622</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>2</v>
@@ -916,7 +871,7 @@
       <c r="A59" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B59" s="11" t="n">
+      <c r="B59" s="10" t="n">
         <f aca="false">B58/B6</f>
         <v>16.5</v>
       </c>
@@ -928,9 +883,9 @@
       <c r="A60" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="12" t="n">
+      <c r="B60" s="11" t="n">
         <f aca="false">B17+B35+B54</f>
-        <v>68.1227618413237</v>
+        <v>65.6005753016622</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>2</v>
@@ -943,18 +898,18 @@
       <c r="A61" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B61" s="13" t="n">
+      <c r="B61" s="12" t="n">
         <f aca="false">B60*B24</f>
-        <v>30.3225810749389</v>
+        <v>29.9270671673714</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B65" s="14" t="n">
+      <c r="B65" s="13" t="n">
         <f aca="false">2*(B4+B22+B40)</f>
-        <v>11571008.25941</v>
+        <v>11740491.743854</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>2</v>
@@ -967,9 +922,9 @@
       <c r="A66" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B66" s="15" t="n">
+      <c r="B66" s="14" t="n">
         <f aca="false">(B65*B24)/1000000</f>
-        <v>5.15044937376441</v>
+        <v>5.35602749488976</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>35</v>
@@ -981,7 +936,7 @@
       </c>
       <c r="B68" s="0" t="n">
         <f aca="false">B9+B27+B46</f>
-        <v>9.89</v>
+        <v>9.18</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>35</v>
@@ -991,122 +946,9 @@
       <c r="A70" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="16" t="n">
+      <c r="B70" s="15" t="n">
         <f aca="false">B68/B66</f>
-        <v>1.92022079672856</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I4" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="18" t="n">
-        <f aca="false">Calculator!B6/Equations!B7</f>
-        <v>1.80656621288812</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="18" t="n">
-        <f aca="false">Calculator!B6*Equations!B7</f>
-        <v>3.00630683486712</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <f aca="false">2*SQRT(B7)/(1+B7)-1</f>
-        <v>-0.00805094396501782</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="18" t="n">
-        <f aca="false">Calculator!B24/Equations!B7</f>
-        <v>0.345051729655791</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="18" t="n">
-        <f aca="false">Calculator!B24*Equations!B7</f>
-        <v>0.574200583320201</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>47</v>
+        <v>1.7139568474506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>